<commit_message>
Fix update Enemy ----- After hosting enemy now goes back to correct position
</commit_message>
<xml_diff>
--- a/Base/TileMap/Level3.xlsx
+++ b/Base/TileMap/Level3.xlsx
@@ -866,21 +866,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BE51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AI19" sqref="AI19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AS14" sqref="AS14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="34" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="4.28515625" customWidth="1"/>
-    <col min="36" max="57" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="57" width="2.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:57" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1053,7 +1048,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1226,7 +1221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1371,11 +1366,11 @@
       <c r="AV3">
         <v>0</v>
       </c>
-      <c r="AW3">
-        <v>0</v>
-      </c>
-      <c r="AX3" s="1">
-        <v>1</v>
+      <c r="AW3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AX3">
+        <v>0</v>
       </c>
       <c r="AY3">
         <v>0</v>
@@ -1399,7 +1394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -1544,11 +1539,11 @@
       <c r="AV4">
         <v>0</v>
       </c>
-      <c r="AW4">
-        <v>0</v>
-      </c>
-      <c r="AX4" s="1">
-        <v>1</v>
+      <c r="AW4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AX4" s="6">
+        <v>0</v>
       </c>
       <c r="AY4" s="6">
         <v>0</v>
@@ -1572,7 +1567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -1717,13 +1712,13 @@
       <c r="AV5">
         <v>0</v>
       </c>
-      <c r="AW5">
-        <v>0</v>
-      </c>
-      <c r="AX5" s="1">
-        <v>1</v>
-      </c>
-      <c r="AY5" s="6">
+      <c r="AW5" s="1">
+        <v>1</v>
+      </c>
+      <c r="AX5" s="6">
+        <v>0</v>
+      </c>
+      <c r="AY5" s="4">
         <v>0</v>
       </c>
       <c r="AZ5" s="4">
@@ -1745,7 +1740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -1890,13 +1885,13 @@
       <c r="AV6">
         <v>0</v>
       </c>
-      <c r="AW6">
-        <v>0</v>
-      </c>
-      <c r="AX6" s="1">
-        <v>1</v>
-      </c>
-      <c r="AY6" s="6">
+      <c r="AW6" s="1">
+        <v>1</v>
+      </c>
+      <c r="AX6" s="6">
+        <v>0</v>
+      </c>
+      <c r="AY6" s="4">
         <v>0</v>
       </c>
       <c r="AZ6" s="4">
@@ -1918,7 +1913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -2063,13 +2058,13 @@
       <c r="AV7">
         <v>0</v>
       </c>
-      <c r="AW7">
-        <v>0</v>
-      </c>
-      <c r="AX7" s="1">
-        <v>1</v>
-      </c>
-      <c r="AY7" s="6">
+      <c r="AW7" s="1">
+        <v>1</v>
+      </c>
+      <c r="AX7" s="6">
+        <v>0</v>
+      </c>
+      <c r="AY7" s="4">
         <v>0</v>
       </c>
       <c r="AZ7" s="4">
@@ -2091,7 +2086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -2236,13 +2231,13 @@
       <c r="AV8">
         <v>0</v>
       </c>
-      <c r="AW8">
-        <v>0</v>
-      </c>
-      <c r="AX8" s="1">
-        <v>1</v>
-      </c>
-      <c r="AY8" s="6">
+      <c r="AW8" s="1">
+        <v>1</v>
+      </c>
+      <c r="AX8" s="6">
+        <v>0</v>
+      </c>
+      <c r="AY8" s="4">
         <v>0</v>
       </c>
       <c r="AZ8" s="4">
@@ -2264,7 +2259,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -2409,13 +2404,13 @@
       <c r="AV9">
         <v>0</v>
       </c>
-      <c r="AW9">
-        <v>0</v>
-      </c>
-      <c r="AX9" s="1">
-        <v>1</v>
-      </c>
-      <c r="AY9" s="6">
+      <c r="AW9" s="1">
+        <v>1</v>
+      </c>
+      <c r="AX9" s="6">
+        <v>0</v>
+      </c>
+      <c r="AY9" s="4">
         <v>0</v>
       </c>
       <c r="AZ9" s="4">
@@ -2437,7 +2432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -2573,8 +2568,8 @@
       <c r="AS10">
         <v>0</v>
       </c>
-      <c r="AT10">
-        <v>0</v>
+      <c r="AT10" s="1">
+        <v>1</v>
       </c>
       <c r="AU10" s="1">
         <v>1</v>
@@ -2585,8 +2580,8 @@
       <c r="AW10" s="1">
         <v>1</v>
       </c>
-      <c r="AX10" s="1">
-        <v>1</v>
+      <c r="AX10" s="6">
+        <v>0</v>
       </c>
       <c r="AY10" s="6">
         <v>0</v>
@@ -2610,7 +2605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -2746,20 +2741,20 @@
       <c r="AS11">
         <v>0</v>
       </c>
-      <c r="AT11">
-        <v>0</v>
-      </c>
-      <c r="AU11" s="5">
+      <c r="AT11" s="5">
         <v>14</v>
       </c>
+      <c r="AU11">
+        <v>0</v>
+      </c>
       <c r="AV11">
         <v>0</v>
       </c>
-      <c r="AW11">
-        <v>0</v>
-      </c>
-      <c r="AX11" s="1">
-        <v>1</v>
+      <c r="AW11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AX11">
+        <v>0</v>
       </c>
       <c r="AY11">
         <v>0</v>
@@ -2783,12 +2778,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>1</v>
       </c>
-      <c r="B12">
-        <v>0</v>
+      <c r="B12" s="1">
+        <v>1</v>
       </c>
       <c r="C12" s="1">
         <v>1</v>
@@ -2859,8 +2854,8 @@
       <c r="Y12">
         <v>0</v>
       </c>
-      <c r="Z12">
-        <v>0</v>
+      <c r="Z12" s="5">
+        <v>15</v>
       </c>
       <c r="AA12" s="1">
         <v>1</v>
@@ -2928,17 +2923,17 @@
       <c r="AV12">
         <v>0</v>
       </c>
-      <c r="AW12">
-        <v>0</v>
-      </c>
-      <c r="AX12" s="1">
-        <v>1</v>
+      <c r="AW12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AX12">
+        <v>0</v>
       </c>
       <c r="AY12">
         <v>0</v>
       </c>
-      <c r="AZ12">
-        <v>0</v>
+      <c r="AZ12" s="5">
+        <v>14</v>
       </c>
       <c r="BA12">
         <v>0</v>
@@ -2956,12 +2951,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>1</v>
       </c>
-      <c r="B13">
-        <v>0</v>
+      <c r="B13" s="1">
+        <v>1</v>
       </c>
       <c r="C13" s="1">
         <v>1</v>
@@ -2996,8 +2991,8 @@
       <c r="M13">
         <v>0</v>
       </c>
-      <c r="N13">
-        <v>0</v>
+      <c r="N13" s="2">
+        <v>22</v>
       </c>
       <c r="O13">
         <v>0</v>
@@ -3129,7 +3124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>1</v>
       </c>
@@ -3302,7 +3297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>1</v>
       </c>
@@ -3475,7 +3470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>1</v>
       </c>
@@ -3648,7 +3643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>1</v>
       </c>
@@ -3821,7 +3816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>1</v>
       </c>
@@ -3994,7 +3989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>1</v>
       </c>
@@ -4167,7 +4162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>1</v>
       </c>
@@ -4340,7 +4335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>1</v>
       </c>
@@ -4389,11 +4384,11 @@
       <c r="P21">
         <v>0</v>
       </c>
-      <c r="Q21">
-        <v>0</v>
-      </c>
-      <c r="R21">
-        <v>0</v>
+      <c r="Q21" s="1">
+        <v>1</v>
+      </c>
+      <c r="R21" s="1">
+        <v>1</v>
       </c>
       <c r="S21">
         <v>0</v>
@@ -4513,7 +4508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>1</v>
       </c>
@@ -4562,11 +4557,11 @@
       <c r="P22">
         <v>0</v>
       </c>
-      <c r="Q22">
-        <v>0</v>
-      </c>
-      <c r="R22">
-        <v>0</v>
+      <c r="Q22" s="1">
+        <v>1</v>
+      </c>
+      <c r="R22" s="1">
+        <v>1</v>
       </c>
       <c r="S22">
         <v>0</v>
@@ -4686,7 +4681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>1</v>
       </c>
@@ -4735,11 +4730,11 @@
       <c r="P23">
         <v>0</v>
       </c>
-      <c r="Q23">
-        <v>0</v>
-      </c>
-      <c r="R23">
-        <v>0</v>
+      <c r="Q23" s="1">
+        <v>1</v>
+      </c>
+      <c r="R23" s="1">
+        <v>1</v>
       </c>
       <c r="S23">
         <v>0</v>
@@ -4859,7 +4854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>1</v>
       </c>
@@ -4908,11 +4903,11 @@
       <c r="P24">
         <v>0</v>
       </c>
-      <c r="Q24">
-        <v>0</v>
-      </c>
-      <c r="R24">
-        <v>0</v>
+      <c r="Q24" s="1">
+        <v>1</v>
+      </c>
+      <c r="R24" s="1">
+        <v>1</v>
       </c>
       <c r="S24">
         <v>0</v>
@@ -5032,7 +5027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>1</v>
       </c>
@@ -5078,8 +5073,8 @@
       <c r="O25">
         <v>0</v>
       </c>
-      <c r="P25">
-        <v>0</v>
+      <c r="P25" s="2">
+        <v>22</v>
       </c>
       <c r="Q25" s="1">
         <v>1</v>
@@ -5205,7 +5200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>1</v>
       </c>
@@ -5378,7 +5373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>1</v>
       </c>
@@ -5551,7 +5546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>1</v>
       </c>
@@ -5600,11 +5595,11 @@
       <c r="P28">
         <v>0</v>
       </c>
-      <c r="Q28">
-        <v>0</v>
-      </c>
-      <c r="R28">
-        <v>0</v>
+      <c r="Q28" s="1">
+        <v>1</v>
+      </c>
+      <c r="R28" s="1">
+        <v>1</v>
       </c>
       <c r="S28">
         <v>0</v>
@@ -5724,12 +5719,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>1</v>
       </c>
-      <c r="B29" s="2">
-        <v>22</v>
+      <c r="B29">
+        <v>0</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -5773,11 +5768,11 @@
       <c r="P29">
         <v>0</v>
       </c>
-      <c r="Q29">
-        <v>0</v>
-      </c>
-      <c r="R29">
-        <v>0</v>
+      <c r="Q29" s="1">
+        <v>1</v>
+      </c>
+      <c r="R29" s="1">
+        <v>1</v>
       </c>
       <c r="S29">
         <v>0</v>
@@ -5897,7 +5892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>1</v>
       </c>
@@ -5946,11 +5941,11 @@
       <c r="P30">
         <v>0</v>
       </c>
-      <c r="Q30">
-        <v>0</v>
-      </c>
-      <c r="R30">
-        <v>0</v>
+      <c r="Q30" s="1">
+        <v>1</v>
+      </c>
+      <c r="R30" s="1">
+        <v>1</v>
       </c>
       <c r="S30">
         <v>0</v>
@@ -6070,7 +6065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>1</v>
       </c>
@@ -6098,8 +6093,8 @@
       <c r="I31">
         <v>0</v>
       </c>
-      <c r="J31" s="2">
-        <v>22</v>
+      <c r="J31">
+        <v>0</v>
       </c>
       <c r="K31">
         <v>0</v>
@@ -6243,7 +6238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>1</v>
       </c>
@@ -6416,7 +6411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>1</v>
       </c>
@@ -6531,8 +6526,8 @@
       <c r="AL33">
         <v>0</v>
       </c>
-      <c r="AM33">
-        <v>0</v>
+      <c r="AM33" s="2">
+        <v>22</v>
       </c>
       <c r="AN33">
         <v>0</v>
@@ -6589,7 +6584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>1</v>
       </c>
@@ -6638,11 +6633,11 @@
       <c r="P34">
         <v>0</v>
       </c>
-      <c r="Q34">
-        <v>0</v>
-      </c>
-      <c r="R34">
-        <v>0</v>
+      <c r="Q34" s="1">
+        <v>1</v>
+      </c>
+      <c r="R34" s="1">
+        <v>1</v>
       </c>
       <c r="S34">
         <v>0</v>
@@ -6762,7 +6757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>1</v>
       </c>
@@ -6811,11 +6806,11 @@
       <c r="P35">
         <v>0</v>
       </c>
-      <c r="Q35">
-        <v>0</v>
-      </c>
-      <c r="R35">
-        <v>0</v>
+      <c r="Q35" s="1">
+        <v>1</v>
+      </c>
+      <c r="R35" s="1">
+        <v>1</v>
       </c>
       <c r="S35">
         <v>0</v>
@@ -6935,7 +6930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>1</v>
       </c>
@@ -6984,17 +6979,17 @@
       <c r="P36">
         <v>0</v>
       </c>
-      <c r="Q36">
-        <v>0</v>
-      </c>
-      <c r="R36">
-        <v>0</v>
-      </c>
-      <c r="S36">
-        <v>0</v>
-      </c>
-      <c r="T36">
-        <v>0</v>
+      <c r="Q36" s="1">
+        <v>1</v>
+      </c>
+      <c r="R36" s="1">
+        <v>1</v>
+      </c>
+      <c r="S36" s="1">
+        <v>1</v>
+      </c>
+      <c r="T36" s="1">
+        <v>1</v>
       </c>
       <c r="U36">
         <v>0</v>
@@ -7108,7 +7103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>1</v>
       </c>
@@ -7157,20 +7152,20 @@
       <c r="P37">
         <v>0</v>
       </c>
-      <c r="Q37">
-        <v>0</v>
-      </c>
-      <c r="R37">
-        <v>0</v>
-      </c>
-      <c r="S37">
-        <v>0</v>
-      </c>
-      <c r="T37">
-        <v>0</v>
-      </c>
-      <c r="U37">
-        <v>0</v>
+      <c r="Q37" s="1">
+        <v>1</v>
+      </c>
+      <c r="R37" s="1">
+        <v>1</v>
+      </c>
+      <c r="S37" s="1">
+        <v>1</v>
+      </c>
+      <c r="T37" s="1">
+        <v>1</v>
+      </c>
+      <c r="U37" s="1">
+        <v>1</v>
       </c>
       <c r="V37">
         <v>0</v>
@@ -7281,7 +7276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>1</v>
       </c>
@@ -7339,8 +7334,8 @@
       <c r="S38">
         <v>0</v>
       </c>
-      <c r="T38">
-        <v>0</v>
+      <c r="T38" s="1">
+        <v>1</v>
       </c>
       <c r="U38" s="1">
         <v>1</v>
@@ -7454,7 +7449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>1</v>
       </c>
@@ -7491,8 +7486,8 @@
       <c r="L39">
         <v>0</v>
       </c>
-      <c r="M39">
-        <v>0</v>
+      <c r="M39" s="2">
+        <v>22</v>
       </c>
       <c r="N39">
         <v>0</v>
@@ -7627,7 +7622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>1</v>
       </c>
@@ -7800,7 +7795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>1</v>
       </c>
@@ -7973,7 +7968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>1</v>
       </c>
@@ -8146,7 +8141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>1</v>
       </c>
@@ -8204,8 +8199,8 @@
       <c r="S43">
         <v>0</v>
       </c>
-      <c r="T43">
-        <v>0</v>
+      <c r="T43" s="2">
+        <v>22</v>
       </c>
       <c r="U43" s="1">
         <v>1</v>
@@ -8319,7 +8314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>1</v>
       </c>
@@ -8492,7 +8487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>1</v>
       </c>
@@ -8665,7 +8660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>1</v>
       </c>
@@ -8838,7 +8833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>1</v>
       </c>
@@ -9011,7 +9006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>1</v>
       </c>
@@ -9184,7 +9179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>1</v>
       </c>
@@ -9357,7 +9352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>1</v>
       </c>
@@ -9370,8 +9365,8 @@
       <c r="D50" s="1">
         <v>1</v>
       </c>
-      <c r="E50" s="3">
-        <v>26</v>
+      <c r="E50">
+        <v>0</v>
       </c>
       <c r="F50">
         <v>0</v>
@@ -9530,7 +9525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>1</v>
       </c>

</xml_diff>